<commit_message>
Changes done Monday morning Allan
</commit_message>
<xml_diff>
--- a/Makaia/data/CreateLead.xlsx
+++ b/Makaia/data/CreateLead.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10311"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{EA406F8F-4EEA-4693-AF75-4F72A773C4AE}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{815C78CA-13B9-D242-BB89-E297465AFC3F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">Company </t>
   </si>
@@ -50,45 +50,6 @@
   </si>
   <si>
     <t>1322221212</t>
-  </si>
-  <si>
-    <t>Allen</t>
-  </si>
-  <si>
-    <t>Bro</t>
-  </si>
-  <si>
-    <t>Allen.bro@games.com</t>
-  </si>
-  <si>
-    <t>3456765445</t>
-  </si>
-  <si>
-    <t>Mani</t>
-  </si>
-  <si>
-    <t>Solamen</t>
-  </si>
-  <si>
-    <t>Manisolamen7@outlook.com</t>
-  </si>
-  <si>
-    <t>9442780472</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TL </t>
-  </si>
-  <si>
-    <t>Sreejith</t>
-  </si>
-  <si>
-    <t>BRo</t>
-  </si>
-  <si>
-    <t>sreejith@tl.co</t>
-  </si>
-  <si>
-    <t>6552656565</t>
   </si>
 </sst>
 </file>
@@ -418,20 +379,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -448,7 +409,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -463,65 +424,11 @@
       </c>
       <c r="E2" s="2" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{856FCF87-D5F3-4A24-BA6B-805289ABFBED}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{D6DEBE77-F8B2-482D-8FE4-C9D13F55CBC5}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{7CB49412-7463-46CE-ACD1-52C12ACCE54D}"/>
-    <hyperlink ref="D5" r:id="rId4" xr:uid="{802F7DB2-239A-40ED-944A-430144EB1AE7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>